<commit_message>
changes from awhile ago
</commit_message>
<xml_diff>
--- a/songlist.xlsx
+++ b/songlist.xlsx
@@ -10,201 +10,190 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="C6">
-      <text>
-        <t xml:space="preserve">Responder updated this value.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D6">
-      <text>
-        <t xml:space="preserve">Responder updated this value.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="E6">
-      <text>
-        <t xml:space="preserve">Responder updated this value.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="F6">
-      <text>
-        <t xml:space="preserve">Responder updated this value.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="G6">
-      <text>
-        <t xml:space="preserve">Responder updated this value.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Timestamp</t>
   </si>
   <si>
-    <t>What is your name?</t>
-  </si>
-  <si>
-    <t>Enter song #1</t>
-  </si>
-  <si>
-    <t>Enter song #2</t>
-  </si>
-  <si>
-    <t>Enter song #3</t>
-  </si>
-  <si>
-    <t>Enter song #4</t>
-  </si>
-  <si>
-    <t>Enter song #5</t>
+    <t>What Is Your Name?</t>
+  </si>
+  <si>
+    <t>Enter Song #1</t>
+  </si>
+  <si>
+    <t>Enter Song #2</t>
+  </si>
+  <si>
+    <t>Enter Song #3</t>
+  </si>
+  <si>
+    <t>Enter Song #4</t>
+  </si>
+  <si>
+    <t>Enter Song #5</t>
+  </si>
+  <si>
+    <t>Trenton</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/0xMEF2WiqKWTIG7Krjungw?si=a6lJ3PuRTBm8UiW1rODWOw</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/5IyL3XOaRPpTgxVjRIAxXU?si=79mxV9hxSvyWqE64r3kkEg</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/0Y9z2PrmiVkFRg1cjtY4cZ?si=0N9jwEWrQDCA_ywYY87O0A</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/6VoIBz0VhCyz7OdEoRYDiA?si=uKkzyJ3BTt6VRt-CEQdKig</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/4GIJ1q3rOtp3Dv3IxwcPHB?si=sVSBLB8kSJSFLEa7UyxqDg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evalyn </t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/6bLU8e0LGyztE9iD5DWBQ1?si=P5sdvN6PQ3uyIvgmN_sKOA&amp;context=spotify%3Aplaylist%3A3IILyTGVqFi6pLky65b7H3</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/2KN0Kgfb15aNLR0p2J4pkr?si=NTe0dvYwQpmS4vW9oEz0Gg&amp;context=spotify%3Aplaylist%3A37i9dQZF1DZ06evO2OtQSh</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/2JXiyD1zucGdFmnTeYb5Ry?si=aWC2e8WjSjOERmUoQazZMQ</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/3Z2anmIVG8b1GelyeFQdnP?si=iQVVgH-JQ46K4496PGk0pw</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/6Qyc6fS4DsZjB2mRW9DsQs?si=OzG1skbwTRCmuErWBBurVQ</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/3KFNeTh4wtw7RMRoSBPqHF?si=YrBW0ZuBRRuEFrR4D73K-g</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/4iya38ctQ1httyA6NOG9oW?si=-oxZ8DNdS2mi1Gqr5WPB8g</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/2fuilieQ5gCZYitFDWt5No?si=YS1vPxZHQKmJ8LszfYIWXQ</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/1W5W3zTbD9yJZJJSzybZlG?si=SmflT4dDR-Osru5I-hNplg</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/02UctveK9r8fS7EApR7zJr?si=CDgY7nF7RUihknxChsTEzg</t>
   </si>
   <si>
     <t>Todd</t>
   </si>
   <si>
-    <t>https://open.spotify.com/track/5267gVdYWrLoz6ClOhlqmE?si=giMQe3viSI25IkLgWTuvhA&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/6TPMFSJFmyIohTM5El90Po?si=suTamx2TTLWruyMM5whRJQ&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/4ByEFOBuLXpCqvO1kw8Wdm?si=EXw254Z4TkmvxLyMH0Y4zw&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/6bx8SPmwSnpAZhLlbeR7vb?si=UXtzdt5KSQyY_n5nK_TswQ&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/6DiPkm7C3LD9XsJWTGPFgv?si=25YEk4BFQPeA6Aqj9FUaqQ&amp;dl_branch=1</t>
+    <t>https://open.spotify.com/track/4ReyTz0y3TGkX48wO3Llot?si=qomYZUeZRbauHcpiHkZTnQ</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/4I3VMhZDVr12BW2VCslDXm?si=WbuzLK-dTWKkjoM1nTH-KQ</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/0KXYrQAqpAREiCi4pB5fO9?si=M582lz3MTwOgesJKl3NoYA</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/7txxAtOMwLLnQTpKeBL6bp?si=0lWp1EcNSKCchgvi_tH5Bg</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/4qM461TqtpnP4GLRIXwEnW?si=LREyDfEJQHGyLARDV67b4w</t>
   </si>
   <si>
     <t>Sheree</t>
   </si>
   <si>
-    <t>https://open.spotify.com/track/6UQkKezR70jMXymMJgRcOz?si=vsRZZcA0RPW4p7PtJllKjw&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/2Raz3qhlFGMQWscZhWkNCV?si=tKg0TINrQHKUkqQNKuTEyA&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/75UvFUebxOBj5Fl5euUqQA?si=2rMTQZo6QhWPhuD6gAMOsg&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/4cgZEMKdekAOLjSvTafZrr?si=5dCIYP2WQ-G3Yt5VYx-75g&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/63vL5oxWrlvaJ0ayNaQnbX?si=0cHKWE2WTr2qckWZgf__2w&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>Rachel</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/7mEDVrAHDnQJStDo8jKJJm?si=iNE89MmFTcSMzRuYBHXZmA&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/63vL5oxWrlvaJ0ayNaQnbX?si=1D6IKFtzRvWBgRouk-L2ug&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/4cOdK2wGLETKBW3PvgPWqT?si=8v0dsOSBRtiOVDTkCUu7WA&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/5aszL9hl6SBzFNsOvw8u8w?si=z2IEihfnTcOfsPTDqZZjjg&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>Trenton</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/1Nz4KHTLNnnc2Wl6teppUR?si=dPu57DWTRqmg6J-lVRfsJw&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/6jO8FdgfPLjcesTmRpFCPX?si=JDfZYGEVT3W8m5T0mrq6RQ&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/3YmFlUmOV28Sf14lJp1QDF?si=6v_2nOs0RhmO_VRqKx3mRA&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/6FQfR11c7domNF662OE14T?si=wNUKvUz9QVmmEQkNa9GdQw&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>Kathy</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/29HaKOpeLSYvqdFyEQSRdj?si=c0cb4b01dbdf4cd6</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/41gyi3lBZzLRiHwfAAoI1G?si=94b540134afa4a44</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/0GONea6G2XdnHWjNZd6zt3?si=eacdc251c3d04869</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/2Y90nL1ohB4sgYELDs7uNx?si=66cddb9c9061483f</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/0hm8rgOY17z7kQJlqGKbu7?si=714297d4234c4c49</t>
+    <t>https://open.spotify.com/track/4ReyTz0y3TGkX48wO3Llot?si=_DzfIAQYQ8Kmj1RcmM-b8A&amp;context=spotify%3Aartist%3A6GbCJZrI318Ybm8mY36Of5</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/4ok8REUtvjCupFwQtj9D5n?si=xnXsNyKFRgiioMzz65q78A</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/5n1AwNQBbWEf6Yq9qJzyBJ?si=ciqYCecJS1aLdzL-Uu-Zug</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/6eddGe0Mn5zDIFnl0HJKr3?si=FQ36Vb95TBGyfiMhT7Tb8w</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/01EBzwufAS0XnF5oGLKgWj?si=s3hnYjdNRsyI1LFwjZKzzw</t>
+  </si>
+  <si>
+    <t>Maggy</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/6GtOsEzNUhJghrIf6UTbRV?si=ZBkzhTDmQemY3CrBWfdQTQ</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/4dXsEEQarPsh8udGfRUE30?si=8sHOa3B5T3KS178Q9s3aRA</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/11dxtPJKR4E0wlSr0A0t47?si=GaXwhtw1R1i_EhbfF7YUDQ</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/1wyluqXP2ujdTpCfm1E617?si=n0HMBAWFRTG1exFaQpzzwA</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/2BstRQGodshjGpeDGQiNgo?si=xwphreLWTxiVOzwPV32O0g</t>
   </si>
   <si>
     <t>Richard</t>
   </si>
   <si>
-    <t>https://open.spotify.com/track/2qK6fxHA2V8mCK9pHry3wa?si=IpgUN1G4QUiEery3YkC6zg&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/2QXLECDuQIRDFb3cRtyp9p?si=CS-NjY3PTPm8fiWEFjHeMg&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/4DEcdqqKokU7UAE4wCGQEy?si=ozMPUt4UTca2smkdh6xZuQ&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/1exUq8aG2OMbSeZeTwz06k?si=0h9NAPLYQ8aabUUMOv76-g&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/6hHUiDe461VUoTHnsplRYs?si=gHZPBaEsSPKibdWW9RCz6A&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>Evalyn</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/5AmzmWV5W2cGE3pHesHMmS?si=62DwOrr7SQevV6XYBkuSfw&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/755inykyaG4w22GWAsA3MX?si=_OcEL2CRRjaiXXWthdKdNQ&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/40riOy7x9W7GXjyGp4pjAv?si=ZuPgQFnaSMOvltpBqOoQAg&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/33OeHNGJA124QytVD0BeQK?si=qDSn8UYgSbmOfg-ZZjMQgg&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/35r28RDot7nPE7y9K9H7l0?si=x7A3n1voTMCR0CgTb-6eqQ&amp;dl_branch=1</t>
+    <t>https://open.spotify.com/track/01E97908af7cRmFC9XXekH?si=8nFgdsAsSLCQRBc-uWMxBw</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/4wO69mm6o7zhaZqSX7YETw?si=fDpOsX33QNGlTxud2dywkA</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/7snQQk1zcKl8gZ92AnueZW?si=HonxahEaSfCalI0wg2Gk0Q</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/57JVGBtBLCfHw2muk5416J?si=AO8OKDCvSZeXHdr0dTUB4g</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/63OQupATfueTdZMWTxW03A?si=bFG9XkXUQgmEov8G21azvQ</t>
   </si>
   <si>
     <t>Shawn</t>
   </si>
   <si>
-    <t>https://open.spotify.com/track/2w3ScXudq4aD3K5HFO5xvx?si=OGcTtn0FQUKJiOPTG7HwHw&amp;utm_source=copy-link&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/1bNVtTNLgeOVgWUqBdXwyP?si=rZXC37gFT-WdKBeFA36D_w&amp;utm_source=native-share-menu&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/2N0volXQpwsvjDorTTxBAU?si=S2-YXBrbQmatkKuLhRaU5Q&amp;utm_source=copy-link&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/album/31M6xnqksyqCJazdzP46iQ?si=NTu5N-OuRm2LHhXXdbGmig&amp;utm_source=copy-link&amp;dl_branch=1</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/track/6iIE4nPK7daEqE3kOC5AP2?si=TCZ5HDa7TNG0k_TZx0B_rA&amp;utm_source=copy-link&amp;dl_branch=1</t>
+    <t>https://open.spotify.com/track/60IGhnH20N82dNxKnc8jDd?si=nPqILTeEQn-Bd_RqAb9XjA&amp;utm_source=copy-link</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://open.spotify.com/playlist/2sF3XmKykZyV3K3b2cS77T?si=ArQIboTvS6uA_FseC89QIA&amp;utm_source=copy-link</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/7nfiM8DuaSJ61KaerHchcA?si=EbqfM44pTtetGojI6wPK9w&amp;utm_source=copy-link&amp;context=spotify%3Aplaylist%3A37i9dQZF1DWWiDhnQ2IIru</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/4RiC0i1VIybdCtTIVhqVVH?si=wt81BeqxQJ2RtLIOTuoPmA&amp;utm_source=copy-link</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/6QhXQOpyYvbpdbyjgAqKdY?si=PrwUvP2yQDWrouoz80P4iQ&amp;utm_source=copy-link&amp;context=spotify%3Aplaylist%3A37i9dQZF1DXa19sXUAHiO1</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/1OolhlC40SrPyo06hQTqXT?si=AQEyiYgiR6WDwnt5ybiWfg</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/55w2MzChxZeTnp45OIm6Ss?si=-chsWy9iTiSWRVQTnQX54g</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/7JIiJLorIcnlvw1yUci492?si=8hWzEwkOQI-vAd8gN2RnEQ</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/6NgRSCfGt18L0ZbpHVBZWW?si=XLLd42MjR4G0flN8PF78wA</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/6JZ8VpAJ6ErPrMtkXjOdcK?si=rq-_uRNeS9iLsnkCzC8PMQ</t>
   </si>
 </sst>
 </file>
@@ -214,21 +203,22 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -244,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -256,12 +246,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -481,9 +465,9 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="13" width="21.57"/>
+    <col customWidth="1" min="1" max="13" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -511,7 +495,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>44380.826033634265</v>
+        <v>44667.8334090625</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -534,7 +518,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>44380.82826380787</v>
+        <v>44667.835824131944</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>13</v>
@@ -557,7 +541,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>44380.82971535879</v>
+        <v>44667.8367034838</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
@@ -572,171 +556,198 @@
         <v>22</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>44380.83098533565</v>
+        <v>44667.83950136574</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5">
-        <v>44380.855592673615</v>
+      <c r="A6" s="2">
+        <v>44667.84029146991</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>44380.84421539352</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>35</v>
+        <v>44667.84275725695</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>44380.84607003472</v>
+        <v>44667.84922520834</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>44380.86150049769</v>
+        <v>44667.85229792824</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>44667.85371594907</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="D2"/>
-    <hyperlink r:id="rId4" ref="E2"/>
-    <hyperlink r:id="rId5" ref="F2"/>
-    <hyperlink r:id="rId6" ref="G2"/>
-    <hyperlink r:id="rId7" ref="C3"/>
-    <hyperlink r:id="rId8" ref="D3"/>
-    <hyperlink r:id="rId9" ref="E3"/>
-    <hyperlink r:id="rId10" ref="F3"/>
-    <hyperlink r:id="rId11" ref="G3"/>
-    <hyperlink r:id="rId12" ref="C4"/>
-    <hyperlink r:id="rId13" ref="D4"/>
-    <hyperlink r:id="rId14" ref="E4"/>
-    <hyperlink r:id="rId15" ref="F4"/>
-    <hyperlink r:id="rId16" ref="G4"/>
-    <hyperlink r:id="rId17" ref="C5"/>
-    <hyperlink r:id="rId18" ref="D5"/>
-    <hyperlink r:id="rId19" ref="E5"/>
-    <hyperlink r:id="rId20" ref="F5"/>
-    <hyperlink r:id="rId21" ref="G5"/>
-    <hyperlink r:id="rId22" ref="C6"/>
-    <hyperlink r:id="rId23" ref="D6"/>
-    <hyperlink r:id="rId24" ref="E6"/>
-    <hyperlink r:id="rId25" ref="F6"/>
-    <hyperlink r:id="rId26" ref="G6"/>
-    <hyperlink r:id="rId27" ref="C7"/>
-    <hyperlink r:id="rId28" ref="D7"/>
-    <hyperlink r:id="rId29" ref="E7"/>
-    <hyperlink r:id="rId30" ref="F7"/>
-    <hyperlink r:id="rId31" ref="G7"/>
-    <hyperlink r:id="rId32" ref="C8"/>
-    <hyperlink r:id="rId33" ref="D8"/>
-    <hyperlink r:id="rId34" ref="E8"/>
-    <hyperlink r:id="rId35" ref="F8"/>
-    <hyperlink r:id="rId36" ref="G8"/>
-    <hyperlink r:id="rId37" ref="C9"/>
-    <hyperlink r:id="rId38" ref="D9"/>
-    <hyperlink r:id="rId39" ref="E9"/>
-    <hyperlink r:id="rId40" ref="F9"/>
-    <hyperlink r:id="rId41" ref="G9"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="D2"/>
+    <hyperlink r:id="rId3" ref="E2"/>
+    <hyperlink r:id="rId4" ref="F2"/>
+    <hyperlink r:id="rId5" ref="G2"/>
+    <hyperlink r:id="rId6" ref="C3"/>
+    <hyperlink r:id="rId7" ref="D3"/>
+    <hyperlink r:id="rId8" ref="E3"/>
+    <hyperlink r:id="rId9" ref="F3"/>
+    <hyperlink r:id="rId10" ref="G3"/>
+    <hyperlink r:id="rId11" ref="C4"/>
+    <hyperlink r:id="rId12" ref="D4"/>
+    <hyperlink r:id="rId13" ref="E4"/>
+    <hyperlink r:id="rId14" ref="F4"/>
+    <hyperlink r:id="rId15" ref="G4"/>
+    <hyperlink r:id="rId16" ref="C5"/>
+    <hyperlink r:id="rId17" ref="D5"/>
+    <hyperlink r:id="rId18" ref="E5"/>
+    <hyperlink r:id="rId19" ref="F5"/>
+    <hyperlink r:id="rId20" ref="G5"/>
+    <hyperlink r:id="rId21" ref="C6"/>
+    <hyperlink r:id="rId22" ref="D6"/>
+    <hyperlink r:id="rId23" ref="E6"/>
+    <hyperlink r:id="rId24" ref="F6"/>
+    <hyperlink r:id="rId25" ref="G6"/>
+    <hyperlink r:id="rId26" ref="C7"/>
+    <hyperlink r:id="rId27" ref="D7"/>
+    <hyperlink r:id="rId28" ref="E7"/>
+    <hyperlink r:id="rId29" ref="F7"/>
+    <hyperlink r:id="rId30" ref="G7"/>
+    <hyperlink r:id="rId31" ref="C8"/>
+    <hyperlink r:id="rId32" ref="D8"/>
+    <hyperlink r:id="rId33" ref="E8"/>
+    <hyperlink r:id="rId34" ref="F8"/>
+    <hyperlink r:id="rId35" ref="G8"/>
+    <hyperlink r:id="rId36" ref="C9"/>
+    <hyperlink r:id="rId37" ref="D9"/>
+    <hyperlink r:id="rId38" ref="E9"/>
+    <hyperlink r:id="rId39" ref="F9"/>
+    <hyperlink r:id="rId40" ref="G9"/>
+    <hyperlink r:id="rId41" ref="C10"/>
+    <hyperlink r:id="rId42" ref="D10"/>
+    <hyperlink r:id="rId43" ref="E10"/>
+    <hyperlink r:id="rId44" ref="F10"/>
+    <hyperlink r:id="rId45" ref="G10"/>
   </hyperlinks>
-  <drawing r:id="rId42"/>
-  <legacyDrawing r:id="rId43"/>
+  <drawing r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>